<commit_message>
interfaz grafica + consulta por nombre de restaurante
</commit_message>
<xml_diff>
--- a/excel/xlsxWrite.xlsx
+++ b/excel/xlsxWrite.xlsx
@@ -14,9 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
-  <si>
-    <t xml:space="preserve"> Lectura actual Lectura anterior Consumo (m3) Vertimiento (m3)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Cod restaurante</t>
+  </si>
+  <si>
+    <t>Lectura actual</t>
+  </si>
+  <si>
+    <t>Lectura anterior</t>
+  </si>
+  <si>
+    <t>Consumo</t>
+  </si>
+  <si>
+    <t>Vertimiento</t>
   </si>
   <si>
     <t>Total a pagar</t>
@@ -351,35 +366,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+      <c r="D2">
+        <v>322</v>
+      </c>
+      <c r="E2">
+        <v>34</v>
+      </c>
+      <c r="F2">
+        <v>34</v>
+      </c>
+      <c r="G2">
+        <v>93000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>492</v>
       </c>
-      <c r="B2">
+      <c r="D3">
         <v>485</v>
       </c>
-      <c r="C2">
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
         <v>43500</v>
       </c>
-      <c r="D2">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
         <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>492</v>
+      </c>
+      <c r="D4">
+        <v>485</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>43500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>492</v>
+      </c>
+      <c r="D5">
+        <v>485</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>43500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>